<commit_message>
REPORTGEN-1177: update STIG-V6 templates config
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Compliance reports/STIG V6 Full Detailed Report.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Compliance reports/STIG V6 Full Detailed Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PJG\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Compliance reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FE184B-EA0F-492C-9353-E2E77E096EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4B06F9-55AA-4B4A-A552-4F084CF8B477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5430" yWindow="2430" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
@@ -144,9 +144,6 @@
     <t>End Line</t>
   </si>
   <si>
-    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE;METRICS=STIG-V5-CAT3,COUNT=-1,HEADER=NO</t>
-  </si>
-  <si>
     <t>Findings summary for CAST under STIG V6</t>
   </si>
   <si>
@@ -187,6 +184,9 @@
   </si>
   <si>
     <t>STIG V6 Compliance details</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE;METRICS=STIG-V6-CAT3,COUNT=-1,HEADER=NO</t>
   </si>
 </sst>
 </file>
@@ -465,20 +465,20 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -857,7 +857,7 @@
   <dimension ref="B1:O15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,12 +883,12 @@
       <c r="E1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="2"/>
@@ -897,12 +897,12 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="2:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="31"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="30"/>
     </row>
     <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="21" t="s">
@@ -974,7 +974,7 @@
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="2:15" ht="22.5" x14ac:dyDescent="0.25">
@@ -993,7 +993,7 @@
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="23"/>
       <c r="D15" s="23"/>
@@ -1028,7 +1028,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1056,7 +1056,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
@@ -1093,7 +1093,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1124,7 +1124,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1152,7 +1152,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1180,7 +1180,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
@@ -1217,7 +1217,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1248,7 +1248,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1276,7 +1276,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1304,7 +1304,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
@@ -1324,7 +1324,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1341,7 +1341,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1372,7 +1372,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>